<commit_message>
Add Upazila data and indicator list
</commit_message>
<xml_diff>
--- a/OutputData/table_format_crop.xlsx
+++ b/OutputData/table_format_crop.xlsx
@@ -1,14 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetamodelTest\OutputData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14355" windowHeight="7995"/>
+    <workbookView xWindow="480" yWindow="72" windowWidth="14352" windowHeight="7992"/>
   </bookViews>
   <sheets>
     <sheet name="crop_loss" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="ESRI_MAPINFO_SHEET" sheetId="4" state="veryHidden" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -96,8 +102,105 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>294147</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>5045</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6390147" cy="1650965"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="none" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>DO NOT EDIT </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="5000" b="1" i="0" cap="none" spc="0">
+              <a:ln w="18000">
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="140000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+                <a:miter lim="800000"/>
+              </a:ln>
+              <a:noFill/>
+              <a:effectLst>
+                <a:outerShdw blurRad="25500" dist="23000" dir="7020000" algn="tl">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="50000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="Verdana" panose="020B0604030504040204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> For Esri use only</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -143,7 +246,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -178,7 +281,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -390,22 +493,22 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.44140625" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -425,7 +528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -445,7 +548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -465,7 +568,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -485,19 +588,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="G13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="G14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="24.6" x14ac:dyDescent="0.3">
       <c r="G16" s="1"/>
     </row>
   </sheetData>
@@ -511,8 +614,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>